<commit_message>
Added Download Transaction Details
</commit_message>
<xml_diff>
--- a/backend/Excels/expense_details.xlsx
+++ b/backend/Excels/expense_details.xlsx
@@ -398,7 +398,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:C2"/>
+  <dimension ref="A1:C11"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -416,18 +416,117 @@
     </row>
     <row r="2">
       <c r="A2" t="str">
+        <v>Drinks</v>
+      </c>
+      <c r="B2">
+        <v>2765</v>
+      </c>
+      <c r="C2" s="1">
+        <v>45991.22928240741</v>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" t="str">
+        <v>Fruits</v>
+      </c>
+      <c r="B3">
+        <v>135</v>
+      </c>
+      <c r="C3" s="1">
+        <v>45989.22928240741</v>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" t="str">
+        <v>Light Bill</v>
+      </c>
+      <c r="B4">
+        <v>586</v>
+      </c>
+      <c r="C4" s="1">
+        <v>45985.22928240741</v>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" t="str">
+        <v>Drinks</v>
+      </c>
+      <c r="B5">
+        <v>1560</v>
+      </c>
+      <c r="C5" s="1">
+        <v>45985.22928240741</v>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" t="str">
+        <v>Birthday Party</v>
+      </c>
+      <c r="B6">
+        <v>2056</v>
+      </c>
+      <c r="C6" s="1">
+        <v>45982.22928240741</v>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" t="str">
+        <v>Dinner</v>
+      </c>
+      <c r="B7">
+        <v>347</v>
+      </c>
+      <c r="C7" s="1">
+        <v>45979.22928240741</v>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" t="str">
+        <v>Fuel</v>
+      </c>
+      <c r="B8">
+        <v>1100</v>
+      </c>
+      <c r="C8" s="1">
+        <v>45979.22928240741</v>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9" t="str">
+        <v>Rent</v>
+      </c>
+      <c r="B9">
+        <v>2400</v>
+      </c>
+      <c r="C9" s="1">
+        <v>45974.22928240741</v>
+      </c>
+    </row>
+    <row r="10">
+      <c r="A10" t="str">
         <v>Bike Servicing</v>
       </c>
-      <c r="B2">
-        <v>1300</v>
-      </c>
-      <c r="C2" s="1">
-        <v>45975.900812789354</v>
+      <c r="B10">
+        <v>1895</v>
+      </c>
+      <c r="C10" s="1">
+        <v>45973.22928240741</v>
+      </c>
+    </row>
+    <row r="11">
+      <c r="A11" t="str">
+        <v>Dinner</v>
+      </c>
+      <c r="B11">
+        <v>462</v>
+      </c>
+      <c r="C11" s="1">
+        <v>45970.22928240741</v>
       </c>
     </row>
   </sheetData>
   <ignoredErrors>
-    <ignoredError numberStoredAsText="1" sqref="A1:C2"/>
+    <ignoredError numberStoredAsText="1" sqref="A1:C11"/>
   </ignoredErrors>
 </worksheet>
 </file>
</xml_diff>